<commit_message>
protected cells in scenarios.xlsx and modelspec.xslx.
</commit_message>
<xml_diff>
--- a/example_data/modelspec.xlsx
+++ b/example_data/modelspec.xlsx
@@ -280,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,6 +296,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -965,13 +977,14 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="17.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="5" width="18.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1017,7 @@
       <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1021,16 +1034,17 @@
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="5" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1049,16 +1063,16 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="19.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="15.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1105,7 @@
       <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1108,11 +1122,12 @@
       <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1193,10 +1208,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="4"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="4"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">

</xml_diff>